<commit_message>
Updated test data of product catalog
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/product_catalog_test_data.xlsx
+++ b/TestData/Web_POS/Billing/product_catalog_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="199" count="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="201" count="299">
   <si>
     <t>TC_Id</t>
   </si>
@@ -611,6 +611,12 @@
   </si>
   <si>
     <t>PC_10</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -691,14 +697,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -720,11 +719,11 @@
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
@@ -1937,7 +1936,7 @@
         <v>198</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
@@ -1946,7 +1945,7 @@
         <v>123456</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>193</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2">
         <v>123456</v>
@@ -1988,13 +1987,13 @@
         <v>25</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="T11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="U11" s="1" t="s">
-        <v>25</v>
+      <c r="U11" s="1">
+        <v>11307101311</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Updated keyword of product catalog
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/product_catalog_test_data.xlsx
+++ b/TestData/Web_POS/Billing/product_catalog_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="201" count="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="202" count="301">
   <si>
     <t>TC_Id</t>
   </si>
@@ -616,7 +616,10 @@
     <t>Copy</t>
   </si>
   <si>
-    <t>0</t>
+    <t>Carry </t>
+  </si>
+  <si>
+    <t>Carry bag</t>
   </si>
 </sst>
 </file>
@@ -1992,8 +1995,8 @@
       <c r="T11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="U11" s="1">
-        <v>11307101311</v>
+      <c r="U11" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>25</v>

</xml_diff>